<commit_message>
added cIAI to framework, prior to changing mortality to not throw out values that don't fit assumption
</commit_message>
<xml_diff>
--- a/Model 1_29/HCUP data.xlsx
+++ b/Model 1_29/HCUP data.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Documents\Carbapenem\Carbapenem-Resistance\Model 1_29\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Documents\Yale\CIDMA\AMR\Carbapenem-Resistance\Model 1_29\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6973AF6B-D821-4622-B9B7-0DA1C66835C8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6750" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6750" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pneumonia" sheetId="1" r:id="rId1"/>
     <sheet name="Sepsis" sheetId="2" r:id="rId2"/>
     <sheet name="UTI" sheetId="3" r:id="rId3"/>
+    <sheet name="cIAI" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="42">
   <si>
     <t>HCUPnet - Hospital Inpatient National Statistics</t>
   </si>
@@ -117,12 +119,42 @@
   </si>
   <si>
     <t>Diagnoses--ICD-9-CM Codes (ICD9), Principal Diagnosis: 038.0  Streptococcal Septicemia, 038.10  Staphylcocc Septicem Nos, 038.19  Staphylcocc Septicem Nec, 038.2  Pneumococcal Septicemia, 038.3  Anaerobic Septicemia, 038.40  Gram-Neg Septicemia Nos, 038.41  H. Influenae Septicemia, 038.42  E Coli Septicemia, 038.43  Pseudomonas Septicemia, 038.44  Serratia Septicemia, 038.49  Gram-Neg Septicemia Nec, 038.8  Septicemia Nec, 038.9  Septicemia Nos, 790.7  Bacteremia, 785.52  Septic Shock, 995.91  Sirs-Infect W/O Org Dysf (after Oct 1, 2006), 995.92  Sirs-Infect W Organ Dysf (after Oct 1, 2006), 038.11  Meth Susc Staph Aur Sept (after Oct 1, 2008), 038.12 Mrsa Septicemia, 038.11  Staph Aureus Septicemia, 995.92 Sirs-Infect W Organ Dysf (after Oct 1, 2006), 995.91  Sirs-Infect W/O Org Dysf, 995.92  Sirs-Infect W Organ Dysf, 785.52 Septic Shock, 995.92 Sirs-Infect W Organ Dysf, 790.7 Bacteremia, 038.1  Staphylococc Septicemia</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Rate of discharges per 100,000 persons</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>†</t>
+  </si>
+  <si>
+    <t>Due to the transition from ICD-9-CM to ICD-10-CM in October 2015, these 2015 statistics were calculated using only quarter 1-3 data, and the statistics available are limited.</t>
+  </si>
+  <si>
+    <t>Rates were calculated using the first three quarters of ICD-9-CM/PCS data for 2015 in the numerator and three-fourths of the national population for 2015 in the denominator</t>
+  </si>
+  <si>
+    <t>Weighted national estimates from HCUP National (Nationwide) Inpatient Sample (NIS), 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, Agency for Healthcare Research and Quality (AHRQ), based on data collected by individual States and provided to AHRQ by the States. Total number of weighted discharges in the U.S. based on HCUP NIS = 35,300,425 (2000); 36,093,550 (2001); 36,523,831 (2002); 37,074,605 (2003); 37,496,978 (2004); 37,843,039 (2005); 38,076,556 (2006); 38,155,908 (2007); 38,210,889 (2008); 37,734,584 (2009); 37,352,013 (2010); 36,962,415 (2011); 36,484,846 (2012); 35,597,792 (2013); 35,358,818 (2014); undefined (2015). Statistics based on estimates with a relative standard error (standard error / weighted estimate) greater than 0.30 or with standard error = 0 in the nationwide statistics (NIS, NEDS, and KID) are not reliable. These statistics are suppressed and are designated with an asterisk (*).</t>
+  </si>
+  <si>
+    <t>Beginning with the 2012 data, the National Inpatient Sample (NIS) was redesigned to optimize national estimates. The nationwide statistics in HCUPnet for years prior to 2012 were regenerated using new trend weights in order to permit longitudinal analysis. The regenerated data were posted to HCUPnet on 7/2/2014. The statistics for years prior to 2012 currently on HCUPnet will differ slightly from statistics obtained prior to 7/2/2014. For more information about the NIS redesign and trend weights, please view the Overview of the NIS.. If you want to use the previous versions of the NIS weights, click here.</t>
+  </si>
+  <si>
+    <t>Analysis Type: Descriptive Statistics | Setting of Care: Hospital Inpatient | Geographic Settings: National | Subgroups of Interest: All Codes Combined, Children only (age 0-17) | Years: 2015, 2014, 2013, 2012, 2011, 2010, 2009, 2008, 2007, 2006, 2005, 2004, 2003, 2002, 2001, 2000 | Categorization Type: Diagnoses--ICD-9-CM Codes (ICD9) | Diagnoses--ICD-9-CM Codes (ICD9): Peritonitis Nos, Peritoneal Abscess, Spontan Bact Peritonitis, Peritonitis Nec, Retroperiton Abscess Nec, Retroperiton Infect Nec | Principal or All-Listed: Principal | Outcome and Measures: Number, Rate</t>
+  </si>
+  <si>
+    <t>Diagnoses--ICD-9-CM Codes (ICD9), Principal Diagnosis: 567.9  Peritonitis Nos, 567.22  Peritoneal Abscess, 567.23  Spontan Bact Peritonitis, 567.38  Retroperiton Abscess Nec, 567.39  Retroperiton Infect Nec, 567.89 Peritonitis Nec, 567.9 Peritonitis Nos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -507,41 +539,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -549,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -557,7 +589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -565,7 +597,7 @@
         <v>1297558.8515164549</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -573,7 +605,7 @@
         <v>1352199.50055038</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -581,7 +613,7 @@
         <v>1298001.3806208761</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -589,7 +621,7 @@
         <v>1187533.2325218297</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -597,7 +629,7 @@
         <v>1165571.2992361053</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -605,7 +637,7 @@
         <v>1213310.2716565763</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -613,7 +645,7 @@
         <v>1266539.9270492154</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -621,7 +653,7 @@
         <v>1174899.8809542293</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -629,7 +661,7 @@
         <v>1306375.6417693391</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -637,7 +669,7 @@
         <v>1186995.2763655467</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -645,7 +677,7 @@
         <v>1154220.9217416123</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -653,7 +685,7 @@
         <v>1153613.3498561326</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -661,7 +693,7 @@
         <v>1155370.2354570525</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -669,7 +701,7 @@
         <v>1102902.8898890109</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -677,7 +709,7 @@
         <v>1148831.6380473822</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -685,7 +717,7 @@
         <v>1103820.3235851068</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -693,7 +725,7 @@
         <v>1074443.7123530649</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -701,17 +733,17 @@
         <v>1012690.3223150712</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -726,41 +758,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B27"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -768,7 +800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -776,7 +808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -784,7 +816,7 @@
         <v>390449.57120550488</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -792,7 +824,7 @@
         <v>386539.04160630942</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -800,7 +832,7 @@
         <v>352953.25632043282</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -808,7 +840,7 @@
         <v>325524.60730293131</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -816,7 +848,7 @@
         <v>331435.71233135043</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -824,7 +856,7 @@
         <v>336875.92968692537</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -832,7 +864,7 @@
         <v>381414.7714077534</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -840,7 +872,7 @@
         <v>442632.10346907139</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -848,7 +880,7 @@
         <v>520163.32446229458</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -856,7 +888,7 @@
         <v>588934.96447570284</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -864,7 +896,7 @@
         <v>654783.89945073694</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -872,7 +904,7 @@
         <v>759644.18485417089</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -880,7 +912,7 @@
         <v>789290.82153466763</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -888,7 +920,7 @@
         <v>883982.42245341849</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -896,7 +928,7 @@
         <v>1041671.2225985825</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -904,7 +936,7 @@
         <v>1127505.2613275275</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -912,7 +944,7 @@
         <v>1290639.5121164261</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -920,17 +952,17 @@
         <v>1507485.4424593372</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -944,41 +976,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -986,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -994,7 +1026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1002,7 +1034,7 @@
         <v>421022.40786991862</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1010,7 +1042,7 @@
         <v>449606.48705764272</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1018,7 +1050,7 @@
         <v>452163.58564050222</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1026,7 +1058,7 @@
         <v>460604.88532644062</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1034,7 +1066,7 @@
         <v>470353.66705525119</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1042,7 +1074,7 @@
         <v>480091.785597938</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1050,7 +1082,7 @@
         <v>515773.3256752353</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1058,7 +1090,7 @@
         <v>532338.08048506302</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1066,7 +1098,7 @@
         <v>554359.31211622362</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1074,7 +1106,7 @@
         <v>559406.16486117139</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1082,7 +1114,7 @@
         <v>566653.80459928559</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1090,7 +1122,7 @@
         <v>612010.42755695095</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1098,7 +1130,7 @@
         <v>627589.42316018871</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1106,7 +1138,7 @@
         <v>658776.53509281971</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +1146,7 @@
         <v>659194.42940306244</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1122,7 +1154,7 @@
         <v>642170.25127604161</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1130,7 +1162,7 @@
         <v>605424.38323379483</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1138,17 +1170,17 @@
         <v>601125.34271259001</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -1159,4 +1191,233 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7312252A-B64E-491E-87D0-7496B803C50F}">
+  <dimension ref="A1:Q32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15:Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>6.9276173622000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>22305.005214438199</v>
+      </c>
+      <c r="C11">
+        <v>6.9952992397999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>23154.9797730926</v>
+      </c>
+      <c r="C12">
+        <v>7.3245388956999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>22415.007358796898</v>
+      </c>
+      <c r="C13">
+        <v>7.1414102010000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>22750.9749060184</v>
+      </c>
+      <c r="C14">
+        <v>7.3017484078999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>22096.1006694725</v>
+      </c>
+      <c r="C15">
+        <v>7.1432985253999997</v>
+      </c>
+      <c r="I15">
+        <v>15557.3475697269</v>
+      </c>
+      <c r="J15">
+        <v>18639.074122518301</v>
+      </c>
+      <c r="K15">
+        <v>19680.573278818702</v>
+      </c>
+      <c r="L15">
+        <v>21540.0273274465</v>
+      </c>
+      <c r="M15">
+        <v>22096.1006694725</v>
+      </c>
+      <c r="N15">
+        <v>22750.9749060184</v>
+      </c>
+      <c r="O15">
+        <v>22415.007358796898</v>
+      </c>
+      <c r="P15">
+        <v>23154.9797730926</v>
+      </c>
+      <c r="Q15">
+        <v>22305.005214438199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>21540.0273274465</v>
+      </c>
+      <c r="C16">
+        <v>7.0215209988999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>19680.573278818702</v>
+      </c>
+      <c r="C17">
+        <v>6.4718723419000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>18639.074122518301</v>
+      </c>
+      <c r="C18">
+        <v>6.1876305273999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>15557.3475697269</v>
+      </c>
+      <c r="C19">
+        <v>5.2139393250000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>